<commit_message>
Edits. add C5 data and debug PROF_to_WPE
</commit_message>
<xml_diff>
--- a/product_data/processing_metadata/C5/PIG_meta.xlsx
+++ b/product_data/processing_metadata/C5/PIG_meta.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kabaldry\OneDrive - University of Tasmania\Documents\Projects\BIO-MATE\BIO-MATE\product_data\processing_metadata\C5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/kimberlee_baldry_utas_edu_au/Documents/Documents/Projects/BIO-MATE/BIO-MATE/product_data/processing_metadata/C5/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4EEF73-6695-4C55-AB0C-5AB074BE5202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B7D7ACF3-C0AE-4A67-A41D-E2D748D3A5A0}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{B7D7ACF3-C0AE-4A67-A41D-E2D748D3A5A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1602,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F66F91E-37FF-4E13-8317-A8978462FC2B}">
   <dimension ref="A1:BU51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>